<commit_message>
#tg-1178 missing views rename column names CLEANUP, ADD documentation
</commit_message>
<xml_diff>
--- a/src/tests/fixtures/views/wms_kaart_database.xlsx
+++ b/src/tests/fixtures/views/wms_kaart_database.xlsx
@@ -18,6 +18,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Blad1!$A$1:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Blad1!$A$1:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Blad1!$A$1:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Blad1!$A$1:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Blad1!$A$1:$J$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t xml:space="preserve">SCHEMA/SERVICE</t>
   </si>
@@ -100,13 +102,7 @@
     <t xml:space="preserve">BGT_PND_pand</t>
   </si>
   <si>
-    <t xml:space="preserve">Ikbestaniet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bal</t>
+    <t xml:space="preserve">identificatie_lokaalid</t>
   </si>
 </sst>
 </file>
@@ -116,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -141,18 +137,141 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFDEADA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFAC090"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFE6E0EC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -163,25 +282,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCC1DA"/>
-        <bgColor rgb="FFB3A2C7"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE6E0EC"/>
-        <bgColor rgb="FFFDEADA"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFDEADA"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFAC090"/>
-        <bgColor rgb="FFCCC1DA"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -191,12 +310,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -207,7 +341,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,103 +365,167 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCC1DA"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFDEADA"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFE6E0EC"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFE6E0EC"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -339,9 +537,9 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFDEADA"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FFB3A2C7"/>
       <rgbColor rgb="FFFAC090"/>
       <rgbColor rgb="FF3366FF"/>
@@ -374,27 +572,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E11" activeCellId="1" sqref="F5:F7 E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="39.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="21.4817813765182"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="20.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="41.246963562753"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="44.4331983805668"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="40.5627530364373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.1943319838057"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="18.165991902834"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="18.6234817813765"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="9.1417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="21.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="41.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="44.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="40.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="23.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="7" width="18.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="7" width="18.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="7" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -617,7 +813,7 @@
         <v>gebouw_vlak&lt;hoogteligging&gt;</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G7" s="5" t="str">
         <f aca="false">C7</f>
@@ -631,38 +827,6 @@
       </c>
       <c r="J7" s="7" t="n">
         <v>3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J8" s="7" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -685,13 +849,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F5:F7 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.79757085020243"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.81"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -711,13 +875,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F5:F7 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.79757085020243"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.81"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>